<commit_message>
bug fixes due to server api changes
</commit_message>
<xml_diff>
--- a/doc/05_Test/Test-Szenarien.xlsx
+++ b/doc/05_Test/Test-Szenarien.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="18915" windowHeight="8250"/>
+    <workbookView xWindow="120" yWindow="100" windowWidth="20060" windowHeight="12900"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="130000"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Szenario</t>
   </si>
@@ -129,12 +134,28 @@
       <t xml:space="preserve"> (DB und Bilder) anzeigen</t>
     </r>
   </si>
+  <si>
+    <t>3. REST Response liefert fehlerhaften output:</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Response liefert HTML Errors</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exception beim Parsen wird abgefangen und evtl. Info message angezeigt</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nein</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,8 +207,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +239,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="27"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -251,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -284,6 +320,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -291,7 +330,7 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -586,22 +625,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1"/>
-    <col min="2" max="2" width="43.5703125" customWidth="1"/>
-    <col min="3" max="3" width="59.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="35.1640625" customWidth="1"/>
+    <col min="2" max="2" width="43.5" customWidth="1"/>
+    <col min="3" max="3" width="59.5" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,7 +655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="33.75" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
@@ -629,7 +669,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="35.25" customHeight="1">
       <c r="A3" s="7"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -641,10 +681,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="D4" s="12"/>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="42">
       <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
@@ -658,7 +698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="65.25" customHeight="1">
       <c r="A6" s="7"/>
       <c r="B6" s="3" t="s">
         <v>12</v>
@@ -670,7 +710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="42">
       <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
         <v>16</v>
@@ -682,32 +722,63 @@
         <v>15</v>
       </c>
     </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
review test cases and fixed trail filtering
</commit_message>
<xml_diff>
--- a/doc/05_Test/Test-Szenarien.xlsx
+++ b/doc/05_Test/Test-Szenarien.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="100" windowWidth="20060" windowHeight="12900"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -41,10 +41,6 @@
     <t>Lokale Daten verfügbar</t>
   </si>
   <si>
-    <t>1. Nur geänderte Daten herunterladen und speichern
-2. Trail-Bilder der geänderten Trails herunterladen und ersetzen</t>
-  </si>
-  <si>
     <t>"Keine Netzwerkverbindung bzw. keine Daten verfügbar"</t>
   </si>
   <si>
@@ -58,10 +54,6 @@
     <t xml:space="preserve">Implementiert? </t>
   </si>
   <si>
-    <t>In Progress
-In Progress</t>
-  </si>
-  <si>
     <t>Beim erstmaligen Starten der Applikation Netzwerk verfügbar, beim nächstmaligen Starten der Applikation kein Netzwerk verfügbar 
 ==&gt; Lokale Daten verfügbar</t>
   </si>
@@ -72,27 +64,7 @@
     <t>Lokale Daten von Internal Storage (DB und Bilder) anzeigen</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Beim erstmaligen Starten der Applikation Netzwerk verfügbar, laufende Applikation verliert aber plötzlich das Netzwerk</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> JA
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>In Progress</t>
-    </r>
   </si>
   <si>
     <r>
@@ -111,8 +83,68 @@
     </r>
   </si>
   <si>
+    <t>3. REST Response liefert fehlerhaften output:</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Response liefert HTML Errors</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exception beim Parsen wird abgefangen und evtl. Info message angezeigt</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nein</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> JA
+ JA</t>
+  </si>
+  <si>
+    <t>1. Nur geänderte Daten herunterladen und speichern
+2. Trail-Bilder der geänderten Trails herunterladen</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Lokale Daten von Internal Storage </t>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> JA</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> JA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lokale Daten von DB </t>
     </r>
     <r>
       <rPr>
@@ -135,27 +167,14 @@
     </r>
   </si>
   <si>
-    <t>3. REST Response liefert fehlerhaften output:</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Response liefert HTML Errors</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exception beim Parsen wird abgefangen und evtl. Info message angezeigt</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nein</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <t>JA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -310,9 +329,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -625,23 +641,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.5" customWidth="1"/>
-    <col min="3" max="3" width="59.5" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" customWidth="1"/>
+    <col min="3" max="3" width="59.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,93 +668,94 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="33.75" customHeight="1">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="35.25" customHeight="1">
+    <row r="3" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="1:4" ht="42">
-      <c r="A5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="65.25" customHeight="1">
+    <row r="6" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>15</v>
+      <c r="D6" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="42">
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>22</v>
+      <c r="C10" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -748,13 +765,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <extLst>
@@ -766,13 +783,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Updated I18N for English Locale
</commit_message>
<xml_diff>
--- a/doc/05_Test/Test-Szenarien.xlsx
+++ b/doc/05_Test/Test-Szenarien.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="19440" windowHeight="12240"/>
+    <workbookView xWindow="7400" yWindow="-420" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Szenario</t>
   </si>
@@ -169,12 +169,36 @@
   <si>
     <t>JA</t>
   </si>
+  <si>
+    <t>4. Detail Ansicht nachdem gefiltert wurde</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Korrekter Trail wird angezeigt</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. Download abbrachen</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vorhandene Internet Verbindung</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trails werden runtergeladen, beim Klick auf Cancel jedoch nicht gespeichert!</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -641,23 +665,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1"/>
-    <col min="2" max="2" width="43.42578125" customWidth="1"/>
-    <col min="3" max="3" width="59.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35.1640625" customWidth="1"/>
+    <col min="2" max="2" width="43.5" customWidth="1"/>
+    <col min="3" max="3" width="59.5" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -671,7 +695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="33.75" customHeight="1">
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
@@ -685,7 +709,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="35.25" customHeight="1">
       <c r="A3" s="7"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -697,10 +721,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="42">
       <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
@@ -714,7 +738,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="65.25" customHeight="1">
       <c r="A6" s="7"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
@@ -726,7 +750,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="42">
       <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
         <v>13</v>
@@ -738,7 +762,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -750,12 +774,33 @@
       </c>
       <c r="D10" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -765,13 +810,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <extLst>
@@ -783,13 +828,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
removed cyclic dependency in package structure
</commit_message>
<xml_diff>
--- a/doc/05_Test/Test-Szenarien.xlsx
+++ b/doc/05_Test/Test-Szenarien.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7400" yWindow="-420" windowWidth="19440" windowHeight="12240"/>
+    <workbookView xWindow="7395" yWindow="-420" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Szenario</t>
   </si>
@@ -81,22 +81,6 @@
       </rPr>
       <t>lokal speichern</t>
     </r>
-  </si>
-  <si>
-    <t>3. REST Response liefert fehlerhaften output:</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Response liefert HTML Errors</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exception beim Parsen wird abgefangen und evtl. Info message angezeigt</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nein</t>
-    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> JA
@@ -171,34 +155,34 @@
   </si>
   <si>
     <t>4. Detail Ansicht nachdem gefiltert wurde</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. REST Response liefert fehlerhaften output:</t>
+  </si>
+  <si>
+    <t>Response liefert HTML Errors</t>
+  </si>
+  <si>
+    <t>Exception beim Parsen wird abgefangen und evtl. Info message angezeigt</t>
+  </si>
+  <si>
+    <t>Vorhandene Internet Verbindung</t>
   </si>
   <si>
     <t>Korrekter Trail wird angezeigt</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>5. Download abbrachen</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vorhandene Internet Verbindung</t>
-    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Trails werden runtergeladen, beim Klick auf Cancel jedoch nicht gespeichert!</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. Download abbrechen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,12 +239,15 @@
       <name val="Verdana"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,12 +269,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="27"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -362,8 +343,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,23 +646,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.5" customWidth="1"/>
-    <col min="3" max="3" width="59.5" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="43" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" customWidth="1"/>
+    <col min="3" max="3" width="59.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -695,7 +676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="33.75" customHeight="1">
+    <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
@@ -706,25 +687,25 @@
         <v>14</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="35.25" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4" ht="42">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
@@ -738,7 +719,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="65.25" customHeight="1">
+    <row r="6" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
@@ -747,60 +728,61 @@
         <v>12</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="42">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+      <c r="D9" s="13"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="D11" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="D13" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -810,13 +792,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <extLst>
@@ -828,13 +810,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>